<commit_message>
RTL Updates:    - fixed compilation errors for timer_nbit    - fixed wrong local param for tmr_32bit module    - fixed various compilation error on mcu_v2
Verification Updates:
   - code cleanup for pwm_tb
   - implemented tb for tmr_nbit
</commit_message>
<xml_diff>
--- a/RTL/Memory/Memory Map.xlsx
+++ b/RTL/Memory/Memory Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosuv\Desktop\Disertatie\RISC-V_Microcontroller\RTL\Memory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E8AB9F-426A-4BCF-A2EB-8377279FC9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919F1785-56E9-4F2F-9B77-376A2D7C254B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{067881A5-A6BC-4587-B776-212172251E8F}"/>
   </bookViews>
@@ -1191,7 +1191,7 @@
   <dimension ref="B1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Script Updates:    -updated assembly.asm code to be able to test the new functionalities    -multiple updates for RV32I assembly script:       1) Implemented support for directly addressing of the SFR of the modules       2) Implemented symbol table for labels       3) Updated the build_* functions to acces symbols from symbol table       4) Implemented support for generating different segments of the code (program+data)       5) Updated logic to generate two bin/hex files for program and data memory    -simplified the memory map (removed some sections of the map, and reduced global data variable     space to be able to acces the entire space without modifying the global pointer during data accesses)
</commit_message>
<xml_diff>
--- a/RTL/Memory/Memory Map.xlsx
+++ b/RTL/Memory/Memory Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosuv\Desktop\Disertatie\RISC-V_Microcontroller\RTL\Memory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919F1785-56E9-4F2F-9B77-376A2D7C254B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83765769-BC66-42DA-B55E-E3FE6BBEA84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{067881A5-A6BC-4587-B776-212172251E8F}"/>
+    <workbookView xWindow="435" yWindow="825" windowWidth="15765" windowHeight="14490" xr2:uid="{067881A5-A6BC-4587-B776-212172251E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>PFM</t>
   </si>
@@ -63,10 +63,6 @@
   </si>
   <si>
     <t>Segment</t>
-  </si>
-  <si>
-    <t>Handlers &amp; ISR
-(~65KB)</t>
   </si>
   <si>
     <t>0xFFFFF800</t>
@@ -88,12 +84,6 @@
     <t>Efective number of instructions</t>
   </si>
   <si>
-    <t>Program:</t>
-  </si>
-  <si>
-    <t>Handlers &amp; ISR:</t>
-  </si>
-  <si>
     <t>Maximum number of Special Function Registers</t>
   </si>
   <si>
@@ -220,10 +210,6 @@
     <t>0x10000000</t>
   </si>
   <si>
-    <t>Program
-(~268MB)</t>
-  </si>
-  <si>
     <t>0x10000FFC</t>
   </si>
   <si>
@@ -234,20 +220,6 @@
 (~4KB)</t>
   </si>
   <si>
-    <t>0xBFFFFFFC</t>
-  </si>
-  <si>
-    <t>0xC0000000</t>
-  </si>
-  <si>
-    <t>Dynamic Data
-(~3GB)</t>
-  </si>
-  <si>
-    <t>Undefined
-(~1GB)</t>
-  </si>
-  <si>
     <t>SFR
 (~2KB)</t>
   </si>
@@ -263,6 +235,21 @@
   </si>
   <si>
     <t>DCO_CNT</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>Program
+(~64KB)</t>
+  </si>
+  <si>
+    <t>Future Expansion
+(~262MB)</t>
+  </si>
+  <si>
+    <t>Future Expansion
+(~3.9GB)</t>
   </si>
 </sst>
 </file>
@@ -286,13 +273,43 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="32">
     <border>
@@ -430,21 +447,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -507,19 +509,6 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -715,11 +704,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -730,11 +745,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -746,112 +757,158 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1190,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{762B2237-A625-460B-A070-D86750612CD8}">
   <dimension ref="B1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,25 +1267,25 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="41"/>
-      <c r="L2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="O2" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="P2" s="33" t="s">
-        <v>54</v>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
+      <c r="L2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="27" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1239,523 +1296,504 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="25"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="34"/>
+        <v>13</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="21"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="28"/>
     </row>
     <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="47" t="s">
+      <c r="B4" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="62" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" s="9">
+        <v>15</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="5">
         <v>0</v>
       </c>
-      <c r="O4" s="11" t="str">
+      <c r="O4" s="7" t="str">
         <f>"0x"&amp;DEC2HEX(HEX2DEC(MID($B$5,3,99))+(N4*4),8)</f>
         <v>0xFFFFF800</v>
       </c>
-      <c r="P4" s="9" t="str">
+      <c r="P4" s="5" t="str">
         <f>O4</f>
         <v>0xFFFFF800</v>
       </c>
     </row>
     <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="30"/>
+      <c r="B5" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="64"/>
+      <c r="D5" s="65"/>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H5">
         <f>(HEX2DEC(MID(B4,3,99))-HEX2DEC(MID(B6,3,99)))/4</f>
         <v>512</v>
       </c>
-      <c r="L5" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="M5" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="21">
+      <c r="L5" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="17">
         <f>N4+1</f>
         <v>1</v>
       </c>
-      <c r="O5" s="23" t="str">
+      <c r="O5" s="19" t="str">
         <f t="shared" ref="O5:O26" si="0">"0x"&amp;DEC2HEX(HEX2DEC(MID($B$5,3,99))+(N5*4),8)</f>
         <v>0xFFFFF804</v>
       </c>
-      <c r="P5" s="24" t="str">
+      <c r="P5" s="20" t="str">
         <f>O5</f>
         <v>0xFFFFF804</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>13</v>
-      </c>
       <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="36"/>
-      <c r="M6" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="N6" s="15">
+        <v>17</v>
+      </c>
+      <c r="L6" s="24"/>
+      <c r="M6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="11">
         <f t="shared" ref="N6:N26" si="1">N5+1</f>
         <v>2</v>
       </c>
-      <c r="O6" s="17" t="str">
+      <c r="O6" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0xFFFFF808</v>
       </c>
-      <c r="P6" s="25"/>
+      <c r="P6" s="21"/>
     </row>
     <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="30"/>
+      <c r="B7" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="58"/>
+      <c r="D7" s="59"/>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H7">
         <f>(HEX2DEC(MID(B6,3,99))-HEX2DEC(MID(B8,3,99)))/4</f>
         <v>512</v>
       </c>
-      <c r="L7" s="36"/>
-      <c r="M7" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="N7" s="15">
+      <c r="L7" s="24"/>
+      <c r="M7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="11">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="O7" s="17" t="str">
+      <c r="O7" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0xFFFFF80C</v>
       </c>
-      <c r="P7" s="25"/>
+      <c r="P7" s="21"/>
     </row>
     <row r="8" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="N8" s="18">
+      <c r="B8" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="40"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" s="14">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="O8" s="20" t="str">
+      <c r="O8" s="16" t="str">
         <f t="shared" si="0"/>
         <v>0xFFFFF810</v>
       </c>
-      <c r="P8" s="26"/>
+      <c r="P8" s="22"/>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="30"/>
-      <c r="L9" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="N9" s="12">
+      <c r="B9" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="41"/>
+      <c r="L9" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" s="8">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="O9" s="14" t="str">
+      <c r="O9" s="10" t="str">
         <f t="shared" si="0"/>
         <v>0xFFFFF814</v>
       </c>
-      <c r="P9" s="24" t="str">
+      <c r="P9" s="20" t="str">
         <f>O9</f>
         <v>0xFFFFF814</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="47" t="s">
+    <row r="10" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="L10" s="36"/>
-      <c r="M10" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="N10" s="15">
+      <c r="L10" s="24"/>
+      <c r="M10" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="N10" s="11">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="O10" s="17" t="str">
+      <c r="O10" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0xFFFFF818</v>
       </c>
-      <c r="P10" s="25"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="46"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="N11" s="15">
+      <c r="P10" s="21"/>
+    </row>
+    <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="52"/>
+      <c r="D11" s="53"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="N11" s="11">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="O11" s="17" t="str">
+      <c r="O11" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0xFFFFF81C</v>
       </c>
-      <c r="P11" s="25"/>
+      <c r="P11" s="21"/>
     </row>
     <row r="12" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="46"/>
+      <c r="B12" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="36"/>
       <c r="F12" t="s">
-        <v>15</v>
-      </c>
-      <c r="L12" s="37"/>
-      <c r="M12" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="N12" s="18">
+        <v>14</v>
+      </c>
+      <c r="L12" s="25"/>
+      <c r="M12" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N12" s="14">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="O12" s="20" t="str">
+      <c r="O12" s="16" t="str">
         <f t="shared" si="0"/>
         <v>0xFFFFF820</v>
       </c>
-      <c r="P12" s="26"/>
+      <c r="P12" s="22"/>
     </row>
     <row r="13" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="30"/>
+      <c r="B13" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="38"/>
+      <c r="D13" s="39"/>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="H13">
-        <f>(HEX2DEC(MID(B14,3,99))-HEX2DEC(MID(B16,3,99)))/4</f>
-        <v>67092480</v>
-      </c>
-      <c r="L13" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="M13" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="N13" s="12">
+        <f>(HEX2DEC(MID(B13,3,99))-HEX2DEC(MID(B15,3,99)))/4</f>
+        <v>16384</v>
+      </c>
+      <c r="L13" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" s="8">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="O13" s="14" t="str">
+      <c r="O13" s="10" t="str">
         <f t="shared" si="0"/>
         <v>0xFFFFF824</v>
       </c>
-      <c r="P13" s="24" t="str">
+      <c r="P13" s="20" t="str">
         <f>O13</f>
         <v>0xFFFFF824</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
-        <v>57</v>
+      <c r="B14" s="42" t="s">
+        <v>6</v>
       </c>
       <c r="C14" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="F14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14">
-        <f>(HEX2DEC(MID(B15,3,99))-HEX2DEC(MID(B17,3,99)))/4</f>
-        <v>16384</v>
-      </c>
-      <c r="L14" s="36"/>
-      <c r="M14" s="16" t="s">
+      <c r="L14" s="24"/>
+      <c r="M14" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="N14" s="11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="O14" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFFFFF828</v>
+      </c>
+      <c r="P14" s="21"/>
+    </row>
+    <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="46"/>
+      <c r="D15" s="47"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N15" s="11">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="O15" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFFFFF82C</v>
+      </c>
+      <c r="P15" s="21"/>
+    </row>
+    <row r="16" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L16" s="25"/>
+      <c r="M16" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="N16" s="14">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="O16" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFFFFF830</v>
+      </c>
+      <c r="P16" s="22"/>
+    </row>
+    <row r="17" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L17" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="M17" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="N14" s="15">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="O14" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>0xFFFFF828</v>
-      </c>
-      <c r="P14" s="25"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="46"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="N15" s="15">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="O15" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>0xFFFFF82C</v>
-      </c>
-      <c r="P15" s="25"/>
-    </row>
-    <row r="16" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="46"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="N16" s="18">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="O16" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>0xFFFFF830</v>
-      </c>
-      <c r="P16" s="26"/>
-    </row>
-    <row r="17" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="30"/>
-      <c r="L17" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="M17" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="N17" s="12">
+      <c r="N17" s="8">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="O17" s="14" t="str">
+      <c r="O17" s="10" t="str">
         <f t="shared" si="0"/>
         <v>0xFFFFF834</v>
       </c>
-      <c r="P17" s="24" t="str">
+      <c r="P17" s="20" t="str">
         <f>O17</f>
         <v>0xFFFFF834</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="L18" s="36"/>
-      <c r="M18" s="16" t="s">
+    <row r="18" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L18" s="24"/>
+      <c r="M18" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="N18" s="11">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="O18" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFFFFF838</v>
+      </c>
+      <c r="P18" s="21"/>
+    </row>
+    <row r="19" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L19" s="24"/>
+      <c r="M19" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N19" s="11">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="O19" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFFFFF83C</v>
+      </c>
+      <c r="P19" s="21"/>
+    </row>
+    <row r="20" spans="12:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L20" s="25"/>
+      <c r="M20" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="N20" s="14">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="O20" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFFFFF840</v>
+      </c>
+      <c r="P20" s="22"/>
+    </row>
+    <row r="21" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L21" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="M21" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="N18" s="15">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="O18" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>0xFFFFF838</v>
-      </c>
-      <c r="P18" s="25"/>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="L19" s="36"/>
-      <c r="M19" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="N19" s="15">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="O19" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>0xFFFFF83C</v>
-      </c>
-      <c r="P19" s="25"/>
-    </row>
-    <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L20" s="37"/>
-      <c r="M20" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="N20" s="18">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="O20" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>0xFFFFF840</v>
-      </c>
-      <c r="P20" s="26"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="L21" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="M21" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="N21" s="21">
+      <c r="N21" s="17">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="O21" s="23" t="str">
+      <c r="O21" s="19" t="str">
         <f t="shared" si="0"/>
         <v>0xFFFFF844</v>
       </c>
-      <c r="P21" s="24" t="str">
+      <c r="P21" s="20" t="str">
         <f>O21</f>
         <v>0xFFFFF844</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="L22" s="36"/>
-      <c r="M22" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="N22" s="15">
+    <row r="22" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L22" s="24"/>
+      <c r="M22" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N22" s="11">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="O22" s="17" t="str">
+      <c r="O22" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0xFFFFF848</v>
       </c>
-      <c r="P22" s="25"/>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="L23" s="36"/>
-      <c r="M23" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="N23" s="15">
+      <c r="P22" s="21"/>
+    </row>
+    <row r="23" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L23" s="24"/>
+      <c r="M23" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="N23" s="11">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="O23" s="17" t="str">
+      <c r="O23" s="13" t="str">
         <f t="shared" si="0"/>
         <v>0xFFFFF84C</v>
       </c>
-      <c r="P23" s="25"/>
-    </row>
-    <row r="24" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L24" s="37"/>
-      <c r="M24" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="N24" s="18">
+      <c r="P23" s="21"/>
+    </row>
+    <row r="24" spans="12:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L24" s="25"/>
+      <c r="M24" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N24" s="14">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="O24" s="20" t="str">
+      <c r="O24" s="16" t="str">
         <f t="shared" si="0"/>
         <v>0xFFFFF850</v>
       </c>
-      <c r="P24" s="26"/>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="L25" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="M25" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="N25" s="12">
+      <c r="P24" s="22"/>
+    </row>
+    <row r="25" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L25" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="M25" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="N25" s="8">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="O25" s="14" t="str">
+      <c r="O25" s="10" t="str">
         <f t="shared" si="0"/>
         <v>0xFFFFF854</v>
       </c>
-      <c r="P25" s="24" t="str">
+      <c r="P25" s="20" t="str">
         <f>O25</f>
         <v>0xFFFFF854</v>
       </c>
     </row>
-    <row r="26" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L26" s="26"/>
-      <c r="M26" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="N26" s="18">
+    <row r="26" spans="12:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L26" s="22"/>
+      <c r="M26" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="N26" s="14">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="O26" s="20" t="str">
+      <c r="O26" s="16" t="str">
         <f t="shared" si="0"/>
         <v>0xFFFFF858</v>
       </c>
-      <c r="P26" s="26"/>
+      <c r="P26" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="29">
@@ -1763,12 +1801,9 @@
     <mergeCell ref="P25:P26"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C16:C17"/>
     <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D17"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D13"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D4:D5"/>
@@ -1788,6 +1823,9 @@
     <mergeCell ref="L13:L16"/>
     <mergeCell ref="L17:L20"/>
     <mergeCell ref="L21:L24"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D10:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Last Push RTL Updates:    - Updated comments    - Updated multiple .f files    - Updated all remaining xls files    - Removed sfr_map.sv component because it was not used in the end
Verification Updates:
   - Updated .asm tests with headers
</commit_message>
<xml_diff>
--- a/RTL/Memory/Memory Map.xlsx
+++ b/RTL/Memory/Memory Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosuv\Desktop\Disertatie\RISC-V_Microcontroller\RTL\Memory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A374464-052A-4532-B162-31C7AEBB83B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82145BB-38D2-4E45-85D4-1D3E98591175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{067881A5-A6BC-4587-B776-212172251E8F}"/>
+    <workbookView xWindow="10095" yWindow="315" windowWidth="15765" windowHeight="14490" xr2:uid="{067881A5-A6BC-4587-B776-212172251E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -806,7 +806,52 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -830,12 +875,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -860,9 +899,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -874,42 +910,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1247,15 +1247,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{762B2237-A625-460B-A070-D86750612CD8}">
   <dimension ref="B1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="4.140625" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" customWidth="1"/>
@@ -1267,24 +1267,24 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="49"/>
       <c r="L2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="M2" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="50" t="s">
+      <c r="N2" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="O2" s="50" t="s">
+      <c r="O2" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="P2" s="52" t="s">
+      <c r="P2" s="64" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1301,19 +1301,19 @@
       <c r="L3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="49"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="53"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="65"/>
     </row>
     <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="60" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
@@ -1341,8 +1341,8 @@
       <c r="B5" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="48"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="61"/>
       <c r="F5" t="s">
         <v>13</v>
       </c>
@@ -1350,7 +1350,7 @@
         <f>(HEX2DEC(MID(B4,3,99))-HEX2DEC(MID(B6,3,99)))/4</f>
         <v>512</v>
       </c>
-      <c r="L5" s="56" t="s">
+      <c r="L5" s="37" t="s">
         <v>27</v>
       </c>
       <c r="M5" s="18" t="s">
@@ -1373,16 +1373,16 @@
       <c r="B6" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="58" t="s">
         <v>9</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="57"/>
+      <c r="L6" s="38"/>
       <c r="M6" s="12" t="s">
         <v>18</v>
       </c>
@@ -1394,14 +1394,14 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF808</v>
       </c>
-      <c r="P6" s="49"/>
+      <c r="P6" s="31"/>
     </row>
     <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="46"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="59"/>
       <c r="F7" t="s">
         <v>15</v>
       </c>
@@ -1409,7 +1409,7 @@
         <f>(HEX2DEC(MID(B6,3,99))-HEX2DEC(MID(B8,3,99)))/4</f>
         <v>512</v>
       </c>
-      <c r="L7" s="57"/>
+      <c r="L7" s="38"/>
       <c r="M7" s="12" t="s">
         <v>19</v>
       </c>
@@ -1421,17 +1421,17 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF80C</v>
       </c>
-      <c r="P7" s="49"/>
+      <c r="P7" s="31"/>
     </row>
     <row r="8" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="54"/>
-      <c r="L8" s="58"/>
+      <c r="D8" s="35"/>
+      <c r="L8" s="39"/>
       <c r="M8" s="15" t="s">
         <v>20</v>
       </c>
@@ -1443,15 +1443,15 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF810</v>
       </c>
-      <c r="P8" s="31"/>
+      <c r="P8" s="32"/>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="55"/>
-      <c r="L9" s="59" t="s">
+      <c r="C9" s="34"/>
+      <c r="D9" s="36"/>
+      <c r="L9" s="40" t="s">
         <v>28</v>
       </c>
       <c r="M9" s="9" t="s">
@@ -1474,13 +1474,13 @@
       <c r="B10" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="64" t="s">
+      <c r="D10" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="L10" s="57"/>
+      <c r="L10" s="38"/>
       <c r="M10" s="12" t="s">
         <v>22</v>
       </c>
@@ -1492,15 +1492,15 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF818</v>
       </c>
-      <c r="P10" s="49"/>
+      <c r="P10" s="31"/>
     </row>
     <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="65"/>
-      <c r="L11" s="57"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="46"/>
+      <c r="L11" s="38"/>
       <c r="M11" s="12" t="s">
         <v>23</v>
       </c>
@@ -1512,20 +1512,20 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF81C</v>
       </c>
-      <c r="P11" s="49"/>
+      <c r="P11" s="31"/>
     </row>
     <row r="12" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="60"/>
+      <c r="D12" s="41"/>
       <c r="F12" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="58"/>
+      <c r="L12" s="39"/>
       <c r="M12" s="15" t="s">
         <v>24</v>
       </c>
@@ -1537,14 +1537,14 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF820</v>
       </c>
-      <c r="P12" s="31"/>
+      <c r="P12" s="32"/>
     </row>
     <row r="13" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="61"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="42"/>
       <c r="F13" t="s">
         <v>58</v>
       </c>
@@ -1552,7 +1552,7 @@
         <f>(HEX2DEC(MID(B13,3,99))-HEX2DEC(MID(B15,3,99)))/4</f>
         <v>16384</v>
       </c>
-      <c r="L13" s="59" t="s">
+      <c r="L13" s="40" t="s">
         <v>43</v>
       </c>
       <c r="M13" s="9" t="s">
@@ -1575,13 +1575,13 @@
       <c r="B14" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="62" t="s">
+      <c r="D14" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="L14" s="57"/>
+      <c r="L14" s="38"/>
       <c r="M14" s="12" t="s">
         <v>32</v>
       </c>
@@ -1593,15 +1593,15 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF828</v>
       </c>
-      <c r="P14" s="49"/>
+      <c r="P14" s="31"/>
     </row>
     <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="63"/>
-      <c r="L15" s="57"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="44"/>
+      <c r="L15" s="38"/>
       <c r="M15" s="12" t="s">
         <v>33</v>
       </c>
@@ -1613,10 +1613,10 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF82C</v>
       </c>
-      <c r="P15" s="49"/>
+      <c r="P15" s="31"/>
     </row>
     <row r="16" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L16" s="58"/>
+      <c r="L16" s="39"/>
       <c r="M16" s="15" t="s">
         <v>34</v>
       </c>
@@ -1628,10 +1628,10 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF830</v>
       </c>
-      <c r="P16" s="31"/>
+      <c r="P16" s="32"/>
     </row>
     <row r="17" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L17" s="59" t="s">
+      <c r="L17" s="40" t="s">
         <v>44</v>
       </c>
       <c r="M17" s="9" t="s">
@@ -1651,7 +1651,7 @@
       </c>
     </row>
     <row r="18" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L18" s="57"/>
+      <c r="L18" s="38"/>
       <c r="M18" s="12" t="s">
         <v>36</v>
       </c>
@@ -1663,10 +1663,10 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF838</v>
       </c>
-      <c r="P18" s="49"/>
+      <c r="P18" s="31"/>
     </row>
     <row r="19" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L19" s="57"/>
+      <c r="L19" s="38"/>
       <c r="M19" s="12" t="s">
         <v>37</v>
       </c>
@@ -1678,10 +1678,10 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF83C</v>
       </c>
-      <c r="P19" s="49"/>
+      <c r="P19" s="31"/>
     </row>
     <row r="20" spans="12:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L20" s="58"/>
+      <c r="L20" s="39"/>
       <c r="M20" s="15" t="s">
         <v>38</v>
       </c>
@@ -1693,10 +1693,10 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF840</v>
       </c>
-      <c r="P20" s="31"/>
+      <c r="P20" s="32"/>
     </row>
     <row r="21" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L21" s="56" t="s">
+      <c r="L21" s="37" t="s">
         <v>45</v>
       </c>
       <c r="M21" s="18" t="s">
@@ -1716,7 +1716,7 @@
       </c>
     </row>
     <row r="22" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L22" s="57"/>
+      <c r="L22" s="38"/>
       <c r="M22" s="12" t="s">
         <v>40</v>
       </c>
@@ -1728,10 +1728,10 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF848</v>
       </c>
-      <c r="P22" s="49"/>
+      <c r="P22" s="31"/>
     </row>
     <row r="23" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L23" s="57"/>
+      <c r="L23" s="38"/>
       <c r="M23" s="12" t="s">
         <v>41</v>
       </c>
@@ -1743,10 +1743,10 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF84C</v>
       </c>
-      <c r="P23" s="49"/>
+      <c r="P23" s="31"/>
     </row>
     <row r="24" spans="12:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L24" s="58"/>
+      <c r="L24" s="39"/>
       <c r="M24" s="15" t="s">
         <v>42</v>
       </c>
@@ -1758,7 +1758,7 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF850</v>
       </c>
-      <c r="P24" s="31"/>
+      <c r="P24" s="32"/>
     </row>
     <row r="25" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L25" s="30" t="s">
@@ -1781,7 +1781,7 @@
       </c>
     </row>
     <row r="26" spans="12:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L26" s="31"/>
+      <c r="L26" s="32"/>
       <c r="M26" s="15" t="s">
         <v>57</v>
       </c>
@@ -1793,23 +1793,10 @@
         <f t="shared" si="0"/>
         <v>0xFFFFF858</v>
       </c>
-      <c r="P26" s="31"/>
+      <c r="P26" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="P13:P16"/>
-    <mergeCell ref="P17:P20"/>
-    <mergeCell ref="P21:P24"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="L5:L8"/>
-    <mergeCell ref="L9:L12"/>
-    <mergeCell ref="L13:L16"/>
-    <mergeCell ref="L17:L20"/>
-    <mergeCell ref="L21:L24"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D10:D11"/>
     <mergeCell ref="L25:L26"/>
     <mergeCell ref="P25:P26"/>
     <mergeCell ref="B2:D2"/>
@@ -1826,6 +1813,19 @@
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="P5:P8"/>
     <mergeCell ref="P9:P12"/>
+    <mergeCell ref="P13:P16"/>
+    <mergeCell ref="P17:P20"/>
+    <mergeCell ref="P21:P24"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="L5:L8"/>
+    <mergeCell ref="L9:L12"/>
+    <mergeCell ref="L13:L16"/>
+    <mergeCell ref="L17:L20"/>
+    <mergeCell ref="L21:L24"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D10:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>